<commit_message>
changed the Method section word count variable to optional
</commit_message>
<xml_diff>
--- a/AssessingRRsPRs_codingscheme_06generalend.xlsx
+++ b/AssessingRRsPRs_codingscheme_06generalend.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
   <si>
     <t>Category</t>
   </si>
@@ -1148,7 +1148,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,6 +1309,9 @@
       </c>
       <c r="F5" t="s">
         <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>39</v>

</xml_diff>